<commit_message>
Update Post-Test Survey Responses.xlsx
</commit_message>
<xml_diff>
--- a/Surveys and Usability Test Documents/Post-Test Survey/Post-Test Survey Responses.xlsx
+++ b/Surveys and Usability Test Documents/Post-Test Survey/Post-Test Survey Responses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Digital-Design-Computer-Organization-VR-Lab\Surveys and Usability Test Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D62B917-9F83-45F0-8069-C1BE3F30E9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F56042-0703-4A4F-99C9-0F1B11B01C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33795" yWindow="2205" windowWidth="22590" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="2550" windowWidth="22590" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -25,43 +25,43 @@
     <t>Timestamp</t>
   </si>
   <si>
-    <t>Did you find it easy to find the required buttons? (1 for very hard and 10 for very easy)</t>
+    <t>Q1. Did you find it easy to find the required buttons? (1 for very hard and 10 for very easy)</t>
   </si>
   <si>
     <t>Any comment about the point?</t>
   </si>
   <si>
-    <t>Did you recognize different icons and labels? (1 for very hard and 10 for very easy)</t>
-  </si>
-  <si>
-    <t>Text and colors were easy for the eyes? (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>The application is easy to use with minimum instructions from the tester. (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>Steps are easy to follow, and buttons are easy to remember  (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>You managed to finish the tasks as fast as possible. (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>Everything was clear and easy to preform without frustration (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>You managed to perform well in labs without difficulties in using the VR equipment</t>
-  </si>
-  <si>
-    <t>You managed to perform well in labs by hearing ROBO instructions and following them.</t>
-  </si>
-  <si>
-    <t>ROBO  instructions were clear and easy to follow</t>
-  </si>
-  <si>
-    <t>You found the application interesting. (1 for no and 10 for yes)</t>
-  </si>
-  <si>
-    <t>You found the gamification functions fun and encouraged competitive behavior. . (1 for no and 10 for yes)</t>
+    <t>Q2.  Did you recognize different icons and labels? (1 for very hard and 10 for very easy)</t>
+  </si>
+  <si>
+    <t>Q3. Text and colors were easy for the eyes? (1 for uneasy and 10 for very clear)</t>
+  </si>
+  <si>
+    <t>Q4. The application is easy to use with minimum instructions from the tester. (1 for very hard and 10 for very easy)</t>
+  </si>
+  <si>
+    <t>Q5. Steps are easy to follow, and buttons are easy to remember  (1 for very hard and 10 for very easy)</t>
+  </si>
+  <si>
+    <t>Q6. You managed to finish the tasks as fast as possible. (1 for slow and 10 for very fast)</t>
+  </si>
+  <si>
+    <t>Q7. Everything was clear and easy to preform without frustration (1 for not clear and hard and 10 for very clear and easy)</t>
+  </si>
+  <si>
+    <t>Q8. You managed to perform well in labs without difficulties in using the VR equipment  (1 for difficult and 10 for very easy)</t>
+  </si>
+  <si>
+    <t>Q9. You managed to perform well in labs by hearing ROBO instructions and following them.  (1 for instructions were not clear and 10 for  instructions were very clear)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q10. ROBO  instructions were clear and easy to follow  (1 for hard and 10 for very easy)   </t>
+  </si>
+  <si>
+    <t>Q11. You found the application interesting. (1 for not interesting and 10 for very interesting)</t>
+  </si>
+  <si>
+    <t>Q12. You found the gamification functions fun and encouraged competitive behavior. . (1 for not interested and 10 for very encouraging)</t>
   </si>
   <si>
     <t>-</t>
@@ -439,12 +439,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y15" sqref="Y15"/>
+      <selection pane="bottomLeft" activeCell="AK23" sqref="AK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="41" width="18.85546875" customWidth="1"/>
+    <col min="1" max="29" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>